<commit_message>
feat(api): Add Docker deployment configuration for C# API
- Create multi-stage Dockerfile with ASP.NET 9.0 runtime
- Add docker-compose.yml for production deployment
- Add deploy.sh script for DigitalOcean deployment
- Add test-deploy.sh for local Docker testing
- Create HealthController for Docker health checks
- Add .dockerignore to exclude build artifacts and secrets
- Configure .env.production and .env.test for environment management
- Update .gitignore to protect all environment files
- Fix ASP.NET 9.0 port configuration (8080 instead of 5000)
- Disable HTTPS redirect (no SSL certificates configured yet)
- Add non-root user security in Docker container

Implements deployment infrastructure for Phase 2 (API)
Ready for DigitalOcean droplet deployment
</commit_message>
<xml_diff>
--- a/project-brief/Smart_home_req_draft.xlsx
+++ b/project-brief/Smart_home_req_draft.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anguyen/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fraserbrown/Documents/Programming/Kangan/SmartHomeProject/project-brief/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61FB76EE-AAA3-C34B-91C9-39CCEDB66267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE9E413-AA61-A94A-ACB2-CC427CB5EBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="680" windowWidth="15120" windowHeight="18940" xr2:uid="{D4591B83-22AF-7E4D-BCAD-015AFCF332D8}"/>
+    <workbookView xWindow="38400" yWindow="620" windowWidth="38400" windowHeight="20980" xr2:uid="{D4591B83-22AF-7E4D-BCAD-015AFCF332D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -169,7 +169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +179,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -195,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -207,9 +213,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -549,7 +558,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,12 +570,12 @@
     <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
@@ -583,13 +592,13 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -597,13 +606,13 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -611,13 +620,13 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -625,13 +634,13 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -639,13 +648,13 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -695,11 +704,11 @@
       </c>
     </row>
     <row r="17" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="2:4" ht="68" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
@@ -762,6 +771,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4bbbffe8-721d-489d-9522-69afd7165877" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="19c37c25-20a4-4636-af6e-4fd92d44cc57">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100796224269B83F640B52D51F4897B49E8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="88892698bd3ec24b8f1a16932e908603">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="19c37c25-20a4-4636-af6e-4fd92d44cc57" xmlns:ns3="4bbbffe8-721d-489d-9522-69afd7165877" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac96c336a0746e022cdc178ababc678c" ns2:_="" ns3:_="">
     <xsd:import namespace="19c37c25-20a4-4636-af6e-4fd92d44cc57"/>
@@ -962,34 +991,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4bbbffe8-721d-489d-9522-69afd7165877" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="19c37c25-20a4-4636-af6e-4fd92d44cc57">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2756FAAE-D5A3-4D3E-BC58-FAEA112A8AC5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D27F0B2-0665-4F0E-B74B-499382E9A03B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4bbbffe8-721d-489d-9522-69afd7165877"/>
+    <ds:schemaRef ds:uri="19c37c25-20a4-4636-af6e-4fd92d44cc57"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88B04F7F-82CF-455E-9FCE-2003A7588A88}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88B04F7F-82CF-455E-9FCE-2003A7588A88}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D27F0B2-0665-4F0E-B74B-499382E9A03B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2756FAAE-D5A3-4D3E-BC58-FAEA112A8AC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="19c37c25-20a4-4636-af6e-4fd92d44cc57"/>
+    <ds:schemaRef ds:uri="4bbbffe8-721d-489d-9522-69afd7165877"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>